<commit_message>
[DG22-2617] add step to tear down docker container after test completed and make one test failed to see the result in github workflow
</commit_message>
<xml_diff>
--- a/packages/test/cypress/fixtures/data.xlsx
+++ b/packages/test/cypress/fixtures/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/kororo/repository/dcceew-safeguard-rules-interface/packages/test/cypress/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/kororo/repository/safeguard-github/rules-interface/packages/test/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328F6E45-19F7-2241-A868-56A4B9CAFC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E148D873-6582-2A4B-B3A9-DF89D91A3697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2443,15 +2443,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001F1E234AE2DD64CAC7C4C2A8D43AD9F" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fdfd0681d808c54b86c2d268d3bba2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca5ba3f9-dfeb-4931-84ba-86796a0d6823" xmlns:ns3="0a6f95da-2a98-4fc3-a63b-269af51b7506" xmlns:ns4="9ea08096-1d6a-4225-8886-dcb3dd04c4bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f084bf1f5a61c27721f169ac85480e0" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2740,6 +2731,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F5E14B5-D6EF-401C-82ED-6CA5F26974B2}">
   <ds:schemaRefs>
@@ -2753,14 +2753,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A69F337-BFDC-4B9A-9645-ACD2998E51C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D779FCF-00EF-4E40-96D9-8E341306CAB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2779,4 +2771,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A69F337-BFDC-4B9A-9645-ACD2998E51C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[DG22-2617] update data test
</commit_message>
<xml_diff>
--- a/packages/test/cypress/fixtures/data.xlsx
+++ b/packages/test/cypress/fixtures/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/kororo/repository/safeguard-github/rules-interface/packages/test/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E148D873-6582-2A4B-B3A9-DF89D91A3697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687F6FE3-B355-3D4A-BD04-C2FC189C8214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2443,6 +2443,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001F1E234AE2DD64CAC7C4C2A8D43AD9F" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fdfd0681d808c54b86c2d268d3bba2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca5ba3f9-dfeb-4931-84ba-86796a0d6823" xmlns:ns3="0a6f95da-2a98-4fc3-a63b-269af51b7506" xmlns:ns4="9ea08096-1d6a-4225-8886-dcb3dd04c4bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f084bf1f5a61c27721f169ac85480e0" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2731,15 +2740,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F5E14B5-D6EF-401C-82ED-6CA5F26974B2}">
   <ds:schemaRefs>
@@ -2753,6 +2753,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A69F337-BFDC-4B9A-9645-ACD2998E51C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D779FCF-00EF-4E40-96D9-8E341306CAB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2771,12 +2779,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A69F337-BFDC-4B9A-9645-ACD2998E51C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[DG22-2617] add logging to help us know which fields are being validating by cypress
</commit_message>
<xml_diff>
--- a/packages/test/cypress/fixtures/data.xlsx
+++ b/packages/test/cypress/fixtures/data.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/kororo/repository/safeguard-github/rules-interface/packages/test/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687F6FE3-B355-3D4A-BD04-C2FC189C8214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECCE098-4FA9-B14B-AE52-175731F207D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HVAC1_C" sheetId="1" r:id="rId1"/>
     <sheet name="HVAC1_E" sheetId="4" r:id="rId2"/>
-    <sheet name="HVAC1_E_CLAUSES" sheetId="5" r:id="rId3"/>
-    <sheet name="bca-climate-zone" sheetId="2" r:id="rId4"/>
-    <sheet name="postcode" sheetId="3" r:id="rId5"/>
-    <sheet name="HVAC1_C (2)" sheetId="7" r:id="rId6"/>
-    <sheet name="HVAC1_E (2)" sheetId="8" r:id="rId7"/>
+    <sheet name="bca-climate-zone" sheetId="2" r:id="rId3"/>
+    <sheet name="postcode" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
     <t>Test ID</t>
   </si>
@@ -197,57 +194,6 @@
     <t>HVAC1_E_004</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>clauses</t>
-  </si>
-  <si>
-    <t>In PDRS HVAC1 Implementation Requirements Clause 3 it states that the activity, including the removal of any existing End-User Equipment, must be performed or supervised by a suitably Licensed person in compliance with the relevant standards and legislation.</t>
-  </si>
-  <si>
-    <t>In PDRS HVAC1 Implementation Requirements Clause 2 it states that The New End-User Equipment or replacement End-User Equipment must be installed.</t>
-  </si>
-  <si>
-    <t>In ESS Clause 6.2 it states that an Accredited Certificate Provider may only create Energy Savings Certificates in respect of the Energy Savings for an Implementation where:
-                                  (a) the Accredited Certificate Provider is the Energy Saver for those Energy Savings as at the Implementation Date; and 
-                                  (b) the Accredited Certificate Provider’s Accreditation Date for that Recognised Energy Saving Activity is prior to the Implementation Date.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In PDRS HVAC1 Equipment Requirements Clause 1 it states that the New End-User Equipment or replacement End-User Equipment must be a registered product in the GEMS Registry as complying with the Greenhouse and Energy Minimum Standards (Air Conditioners up to 65kW) Determination 2019.  </t>
-  </si>
-  <si>
-    <t>In ESS Clause 9.9.1E it states that the Accredited Certificate Provider has evidence satisfactory to the Scheme Administrator that the Purchaser has paid for the Implementation, assessment and other associated works carried out at the Site a Net Amount of at least $200 (excluding GST) for each item of End-User Equipment installed as part of an Implementation using any of Activity Definitions F1.1, F1.2, F16 or F17.</t>
-  </si>
-  <si>
-    <t>In PDRS HVAC1 Equipment Requirements Clause 2 it states that if the New End-User Equipment or replacement End-User Equipment has a Cooling Capacity recorded in the GEMS Registry: &lt;br /&gt;\n        a. The New End-User Equipment or replacement End-User Equipment must have a Residential TCSPF_mixed value, as recorded in the GEMS Registry, equal to or greater than the Minimum Residential TCSPF_mixed value for the corresponding Product Type and Cooling Capacity in Table HVAC1.3; or &lt;br /&gt;\n        b. If the New End-User Equipment or replacement End-User Equipment does not have a Residential TCSPF_mixed value recorded in the GEMS Registry, then it must have an AEER in the GEMS Registry equal to or greater than the Minimum AEER for the Product Type and Cooling Capacity in Table HVAC1.4.</t>
-  </si>
-  <si>
-    <t>In PDRS HVAC1 Equipment Requirements Clause 2 it states that if the New End-User Equipment or replacement End-User Equipment has a Cooling Capacity recorded in the GEMS Registry: 
-        a. The New End-User Equipment or replacement End-User Equipment must have a Residential TCSPF_mixed value, as recorded in the GEMS Registry, equal to or greater than the Minimum Residential TCSPF_mixed value for the corresponding Product Type and Cooling Capacity in Table HVAC1.3; or 
-        b. If the New End-User Equipment or replacement End-User Equipment does not have a Residential TCSPF_mixed value recorded in the GEMS Registry, then it must have an AEER in the GEMS Registry equal to or greater than the Minimum AEER for the Product Type and Cooling Capacity in Table HVAC1.4.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In ESS D16 Equipment Requirements Clauses 3 and 4 it states that:
-        3. If the New End-User Equipment or replacement End-User Equipment has a Heating Capacity recorded in the GEMS Registry, and is installed in the hot or average zone as defined in Table A27: 
-          a. It must have a Residential HSPF_mixed value, as recorded in the GEMS Registry, equal to or greater than the Minimum Residential HSPF_mixed value for the same Product Type and Cooling Capacity in Table D16.4; or
-          b. If it does not have a Residential HSPF_mixed value recorded in the GEMS Registry, then it must have a Rated ACOP in the GEMS Registry equal to or greater than the Minimum Rated ACOP for the same Product Type and Cooling Capacity in Table D16.5.
-        4. If the New End-User Equipment or replacement End-User Equipment has a Heating Capacity recorded in the GEMS Registry and is installed in the cold zone as defined in Table A27:
-          a. It must have a Residential HSPF_cold value, as recorded in the GEMS Registry, equal to or greater than the Minimum Residential HSPF_cold value for the same Product Type and Cooling Capacity in Table D16.4; or
-          b. If it does not have a Residential HSPF_cold value recorded in the GEMS Registry, then it must have a Rated ACOP in the GEMS Registry equal to or greater than the Minimum Rated ACOP for the same Product Type and Cooling Capacity in Table D16.5.
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">In ESS D16 Equipment Requirements Clauses 3 and 4 it states that:
-        3. If the New End-User Equipment or replacement End-User Equipment has a Heating Capacity recorded in the GEMS Registry, and is installed in the hot or average zone as defined in Table A27: 
-        a. It must have a Residential HSPF_mixed value, as recorded in the GEMS Registry, equal to or greater than the Minimum Residential HSPF_mixed value for the same Product Type and Cooling Capacity in Table D16.4; or
-        b. If it does not have a Residential HSPF_mixed value recorded in the GEMS Registry, then it must have a Rated ACOP in the GEMS Registry equal to or greater than the Minimum Rated ACOP for the same Product Type and Cooling Capacity in Table D16.5.
-        4. If the New End-User Equipment or replacement End-User Equipment has a Heating Capacity recorded in the GEMS Registry and is installed in the cold zone as defined in Table A27:
-        a. It must have a Residential HSPF_cold value, as recorded in the GEMS Registry, equal to or greater than the Minimum Residential HSPF_cold value for the same Product Type and Cooling Capacity in Table D16.4; or
-        b. If it does not have a Residential HSPF_cold value recorded in the GEMS Registry, then it must have a Rated ACOP in the GEMS Registry equal to or greater than the Minimum Rated ACOP for the same Product Type and Cooling Capacity in Table D16.5.
-        </t>
-  </si>
-  <si>
     <t>BCA_Climate_Zone_2</t>
   </si>
   <si>
@@ -269,27 +215,9 @@
     <t>no</t>
   </si>
   <si>
-    <t>HVAC1_C_004</t>
-  </si>
-  <si>
-    <t>HVAC1_C_005</t>
-  </si>
-  <si>
-    <t>Required Fields</t>
-  </si>
-  <si>
-    <t>requiredFields</t>
-  </si>
-  <si>
     <t>HVAC1_PDRSAug24_Activity</t>
   </si>
   <si>
-    <t>HVAC1_C_006</t>
-  </si>
-  <si>
-    <t>HVAC1_C_007</t>
-  </si>
-  <si>
     <t>HVAC1_PDRSAug24_new_equipment_cooling_capacity,HVAC1_PDRSAug24_AEER_greater_than_minimum,HVAC1_PDRSAug24_new_equipment_heating_capacity</t>
   </si>
   <si>
@@ -357,9 +285,6 @@
   </si>
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>HVAC1_PDRSAug24_new_installation_or_replacement,HVAC1_PDRSAug24_new_installation_or_replacement</t>
   </si>
   <si>
     <t>ineligibleQuestions</t>
@@ -369,7 +294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,13 +306,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -410,13 +328,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -763,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,7 +738,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -834,22 +750,22 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -857,22 +773,22 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C3">
         <v>2800</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="H3">
         <v>23</v>
@@ -892,22 +808,22 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>2000</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -927,22 +843,22 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>2795</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -970,7 +886,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -978,17 +894,17 @@
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="45.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="47.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="48.1640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="44.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="36.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="45.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="47.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="48.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="44.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="36.5" style="2" customWidth="1"/>
     <col min="16" max="16" width="54" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1002,40 +918,40 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1047,49 +963,49 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>46</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
@@ -1097,88 +1013,88 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
       <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6" t="s">
-        <v>98</v>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
@@ -1186,84 +1102,84 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="O6" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1271,133 +1187,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192BC781-DD9B-41E3-9287-CC7A042F5490}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="47.6640625" customWidth="1"/>
-    <col min="2" max="2" width="165.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="112" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="112" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="272" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="272" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="272" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="256" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2786CED2-7BEF-4054-842D-DA68BCCB8D75}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1428,7 +1221,7 @@
         <v>2431</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1436,7 +1229,7 @@
         <v>2890</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1444,7 +1237,7 @@
         <v>2898</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1452,7 +1245,7 @@
         <v>2339</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1460,7 +1253,7 @@
         <v>2342</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1468,7 +1261,7 @@
         <v>2379</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1500,7 +1293,7 @@
         <v>2354</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1508,7 +1301,7 @@
         <v>2359</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1516,7 +1309,7 @@
         <v>2475</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1548,7 +1341,7 @@
         <v>2365</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1556,7 +1349,7 @@
         <v>2624</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1564,12 +1357,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6EC151F-5CD6-4BE1-BB25-71A93C50E291}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1583,7 +1376,7 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1591,7 +1384,7 @@
         <v>2000</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1599,7 +1392,7 @@
         <v>2431</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1607,7 +1400,7 @@
         <v>2890</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1615,7 +1408,7 @@
         <v>2898</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1623,7 +1416,7 @@
         <v>2339</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1631,7 +1424,7 @@
         <v>2342</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1639,7 +1432,7 @@
         <v>2379</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1647,7 +1440,7 @@
         <v>2000</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1655,7 +1448,7 @@
         <v>2128</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1663,7 +1456,7 @@
         <v>2839</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1671,7 +1464,7 @@
         <v>2354</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1679,7 +1472,7 @@
         <v>2359</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1687,7 +1480,7 @@
         <v>2475</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1695,7 +1488,7 @@
         <v>2350</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1703,7 +1496,7 @@
         <v>2368</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1711,7 +1504,7 @@
         <v>2580</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1719,7 +1512,7 @@
         <v>2365</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1727,7 +1520,7 @@
         <v>2624</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1735,7 +1528,7 @@
         <v>3000</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1743,7 +1536,7 @@
         <v>3421</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1751,7 +1544,7 @@
         <v>3519</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1759,7 +1552,7 @@
         <v>4173</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1767,660 +1560,8 @@
         <v>4596</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9C1EEA-4954-8E44-9208-CE3F5C52B99D}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3">
-        <v>2800</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3">
-        <v>23</v>
-      </c>
-      <c r="I3">
-        <v>245</v>
-      </c>
-      <c r="J3">
-        <v>22.01</v>
-      </c>
-      <c r="K3">
-        <v>23.37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>89</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>8.65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5">
-        <v>2795</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3800</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2541</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8">
-        <v>2700</v>
-      </c>
-      <c r="D8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2800</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EBEADA-E54E-3C4F-9EFA-55641646C71D}">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1:Q6"/>
-  <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="45.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="47.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="48.1640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="44.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="36.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="54" style="1" customWidth="1"/>
-    <col min="17" max="17" width="85.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="80" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" s="6"/>
-    </row>
-    <row r="4" spans="1:17" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="Q5" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="O6" s="6"/>
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2443,15 +1584,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001F1E234AE2DD64CAC7C4C2A8D43AD9F" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fdfd0681d808c54b86c2d268d3bba2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca5ba3f9-dfeb-4931-84ba-86796a0d6823" xmlns:ns3="0a6f95da-2a98-4fc3-a63b-269af51b7506" xmlns:ns4="9ea08096-1d6a-4225-8886-dcb3dd04c4bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f084bf1f5a61c27721f169ac85480e0" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2740,6 +1872,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F5E14B5-D6EF-401C-82ED-6CA5F26974B2}">
   <ds:schemaRefs>
@@ -2753,14 +1894,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A69F337-BFDC-4B9A-9645-ACD2998E51C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D779FCF-00EF-4E40-96D9-8E341306CAB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2779,4 +1912,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A69F337-BFDC-4B9A-9645-ACD2998E51C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>